<commit_message>
new function sits_gbm for Gradient Boosting Machine
</commit_message>
<xml_diff>
--- a/inst/extdata/results/embrapa_mt_results_5fold_validation.xlsx
+++ b/inst/extdata/results/embrapa_mt_results_5fold_validation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35880" yWindow="-5280" windowWidth="33640" windowHeight="18400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="35880" yWindow="-5280" windowWidth="33640" windowHeight="18400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="comparacao" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="mlr" sheetId="3" r:id="rId4"/>
     <sheet name="qda" sheetId="4" r:id="rId5"/>
     <sheet name="svm" sheetId="5" r:id="rId6"/>
+    <sheet name="rfor" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="glm_5folds_byclass" localSheetId="1">Lasso!$A$22:$E$36</definedName>
@@ -92,6 +93,18 @@
     <definedName name="qda_relabel2_byclass" localSheetId="4">qda!#REF!</definedName>
     <definedName name="qda_relabel2_overall" localSheetId="4">qda!#REF!</definedName>
     <definedName name="qda_relabel2_table" localSheetId="4">qda!#REF!</definedName>
+    <definedName name="rfor_5folds_byclass" localSheetId="6">rfor!$A$21:$E$35</definedName>
+    <definedName name="rfor_5folds_overall" localSheetId="6">rfor!$A$17:$B$19</definedName>
+    <definedName name="rfor_5folds_table" localSheetId="6">rfor!$A$1:$O$15</definedName>
+    <definedName name="rfor_5foldsreclass_4classes_byclass" localSheetId="6">rfor!$A$95:$E$99</definedName>
+    <definedName name="rfor_5foldsreclass_4classes_overall" localSheetId="6">rfor!$A$91:$B$93</definedName>
+    <definedName name="rfor_5foldsreclass_4classes_table" localSheetId="6">rfor!$A$85:$E$89</definedName>
+    <definedName name="rfor_5foldsreclass_7classes_byclass" localSheetId="6">rfor!$A$75:$E$82</definedName>
+    <definedName name="rfor_5foldsreclass_7classes_overall" localSheetId="6">rfor!$A$71:$B$73</definedName>
+    <definedName name="rfor_5foldsreclass_7classes_table" localSheetId="6">rfor!$A$62:$H$69</definedName>
+    <definedName name="rfor_5foldsreclass_8classes_byclass" localSheetId="6">rfor!$A$52:$E$60</definedName>
+    <definedName name="rfor_5foldsreclass_8classes_overall" localSheetId="6">rfor!$A$48:$B$50</definedName>
+    <definedName name="rfor_5foldsreclass_8classes_table" localSheetId="6">rfor!$A$38:$I$46</definedName>
     <definedName name="svm_5folds_byclass" localSheetId="5">svm!$A$21:$E$35</definedName>
     <definedName name="svm_5folds_overall" localSheetId="5">svm!$A$17:$B$19</definedName>
     <definedName name="svm_5folds_table" localSheetId="5">svm!$A$1:$O$15</definedName>
@@ -104,11 +117,17 @@
     <definedName name="svm_reclass_8classes_byclass_1" localSheetId="5">svm!$A$52:$E$60</definedName>
     <definedName name="svm_reclass_8classes_overall_1" localSheetId="5">svm!$A$48:$B$50</definedName>
     <definedName name="svm_reclass_8classes_table_1" localSheetId="5">svm!$A$38:$I$46</definedName>
+    <definedName name="svm_relabel1_byclass" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel1_byclass" localSheetId="5">svm!#REF!</definedName>
+    <definedName name="svm_relabel1_overall" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel1_overall" localSheetId="5">svm!#REF!</definedName>
+    <definedName name="svm_relabel1_table" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel1_table" localSheetId="5">svm!#REF!</definedName>
+    <definedName name="svm_relabel2_byclass" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel2_byclass" localSheetId="5">svm!#REF!</definedName>
+    <definedName name="svm_relabel2_overall" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel2_overall" localSheetId="5">svm!#REF!</definedName>
+    <definedName name="svm_relabel2_table" localSheetId="6">rfor!#REF!</definedName>
     <definedName name="svm_relabel2_table" localSheetId="5">svm!#REF!</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -941,8 +960,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="73" name="svm_5folds_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_byclass.csv" comma="1">
+  <connection id="73" name="rfor_5folds_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5folds_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -952,16 +971,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="74" name="svm_5folds_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_overall.csv" comma="1">
+  <connection id="74" name="rfor_5folds_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5folds_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="75" name="svm_5folds_table" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_table.csv" comma="1">
+  <connection id="75" name="rfor_5folds_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5folds_table.csv" comma="1">
       <textFields count="15">
         <textField/>
         <textField/>
@@ -981,8 +1000,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="76" name="svm_reclass_4classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_byclass.csv" comma="1">
+  <connection id="76" name="rfor_5foldsreclass_4classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_4classes_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -992,16 +1011,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="77" name="svm_reclass_4classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_overall.csv" comma="1">
+  <connection id="77" name="rfor_5foldsreclass_4classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_4classes_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="78" name="svm_reclass_4classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_table.csv" comma="1">
+  <connection id="78" name="rfor_5foldsreclass_4classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_4classes_table.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -1011,8 +1030,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="79" name="svm_reclass_7classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_byclass.csv" comma="1">
+  <connection id="79" name="rfor_5foldsreclass_7classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_7classes_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -1022,16 +1041,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="80" name="svm_reclass_7classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_overall.csv" comma="1">
+  <connection id="80" name="rfor_5foldsreclass_7classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_7classes_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="81" name="svm_reclass_7classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_table.csv" comma="1">
+  <connection id="81" name="rfor_5foldsreclass_7classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_7classes_table.csv" comma="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -1044,8 +1063,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="82" name="svm_reclass_8classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_byclass.csv" comma="1">
+  <connection id="82" name="rfor_5foldsreclass_8classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_8classes_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -1055,16 +1074,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="83" name="svm_reclass_8classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_overall.csv" comma="1">
+  <connection id="83" name="rfor_5foldsreclass_8classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_8classes_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="84" name="svm_reclass_8classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_table.csv" comma="1">
+  <connection id="84" name="rfor_5foldsreclass_8classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/gilberto/sits/inst/extdata/results/rfor_5foldsreclass_8classes_table.csv" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -1078,8 +1097,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="85" name="svm_relabel1_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_byclass.csv" comma="1">
+  <connection id="85" name="svm_5folds_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -1089,17 +1108,23 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="86" name="svm_relabel1_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_overall.csv" comma="1">
+  <connection id="86" name="svm_5folds_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="87" name="svm_relabel1_table" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_table.csv" comma="1">
-      <textFields count="9">
+  <connection id="87" name="svm_5folds_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_5folds_table.csv" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -1112,8 +1137,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="88" name="svm_relabel2_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel2_byclass.csv" comma="1">
+  <connection id="88" name="svm_reclass_4classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_byclass.csv" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -1123,15 +1148,146 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="89" name="svm_relabel2_overall" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel2_overall.csv" comma="1">
+  <connection id="89" name="svm_reclass_4classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_overall.csv" comma="1">
       <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="90" name="svm_relabel2_table" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="90" name="svm_reclass_4classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_4classes_table.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="91" name="svm_reclass_7classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_byclass.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="92" name="svm_reclass_7classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_overall.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="93" name="svm_reclass_7classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_7classes_table.csv" comma="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="94" name="svm_reclass_8classes_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_byclass.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="95" name="svm_reclass_8classes_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_overall.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="96" name="svm_reclass_8classes_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_reclass_8classes_table.csv" comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="97" name="svm_relabel1_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_byclass.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="98" name="svm_relabel1_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_overall.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="99" name="svm_relabel1_table" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel1_table.csv" comma="1">
+      <textFields count="9">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="100" name="svm_relabel2_byclass" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel2_byclass.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="101" name="svm_relabel2_overall" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel2_overall.csv" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="102" name="svm_relabel2_table" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/gilberto/sits/inst/extdata/results/svm_relabel2_table.csv" comma="1">
       <textFields count="8">
         <textField/>
@@ -1149,7 +1305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="56">
   <si>
     <t>Cerrado</t>
   </si>
@@ -1302,6 +1458,21 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>RFOR Original - 14 classes</t>
+  </si>
+  <si>
+    <t>RFOR - reclass 8 classes</t>
+  </si>
+  <si>
+    <t>RFOR - reclass 7 classes</t>
+  </si>
+  <si>
+    <t>RFOR - reclass 4 classes</t>
+  </si>
+  <si>
+    <t>RFOR</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1884,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable49.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_byclass_1" connectionId="82" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_byclass_1" connectionId="94" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1721,43 +1892,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable50.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_table_1" connectionId="81" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_table_1" connectionId="93" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable51.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_overall_1" connectionId="80" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_overall_1" connectionId="92" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable52.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_byclass_1" connectionId="79" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_7classes_byclass_1" connectionId="91" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable53.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_table_1" connectionId="78" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_table_1" connectionId="90" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable54.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_overall_1" connectionId="77" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_overall_1" connectionId="89" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable55.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_byclass_1" connectionId="76" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_4classes_byclass_1" connectionId="88" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable56.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_table" connectionId="75" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_table" connectionId="87" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable57.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_overall" connectionId="74" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_overall" connectionId="86" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable58.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_byclass" connectionId="73" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_5folds_byclass" connectionId="85" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable59.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_table_1" connectionId="84" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_table_1" connectionId="96" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1765,11 +1936,59 @@
 </file>
 
 <file path=xl/queryTables/queryTable60.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_overall_1" connectionId="83" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="svm_reclass_8classes_overall_1" connectionId="95" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable61.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_4classes_byclass" connectionId="76" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable62.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_4classes_overall" connectionId="77" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable63.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_4classes_table" connectionId="78" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable64.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_7classes_byclass" connectionId="79" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable65.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_7classes_overall" connectionId="80" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable66.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_7classes_table" connectionId="81" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable67.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_8classes_byclass" connectionId="82" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable68.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_8classes_overall" connectionId="83" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable69.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5foldsreclass_8classes_table" connectionId="84" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="glm_reclass_7classes_overall_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable70.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5folds_byclass" connectionId="73" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable71.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5folds_overall" connectionId="74" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable72.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rfor_5folds_table" connectionId="75" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2043,10 +2262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2116,186 +2335,228 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="39">
+        <f>rfor!B18</f>
+        <v>0.74810019701660602</v>
+      </c>
+      <c r="D6" s="39">
+        <f>rfor!B49</f>
+        <v>0.81058260624824097</v>
+      </c>
+      <c r="E6" s="39">
+        <f>rfor!B72</f>
+        <v>0.87925696594427205</v>
+      </c>
+      <c r="F6" s="39">
+        <f>rfor!B92</f>
+        <v>0.92851111736560699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C7" s="39">
         <f>qda!B18</f>
         <v>0.740782437376865</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D7" s="39">
         <f>qda!B49</f>
         <v>0.81593019983112902</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E7" s="39">
         <f>qda!B73</f>
         <v>0.88516746411483205</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F7" s="39">
         <f>qda!B92</f>
         <v>0.932169997185477</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="12" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C8" s="39">
         <f>svm!B18</f>
         <v>0.73290177314945104</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D8" s="39">
         <f>svm!B49</f>
         <v>0.80945679707289597</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E8" s="39">
         <f>svm!B72</f>
         <v>0.87334646777371205</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F8" s="39">
         <f>svm!B92</f>
         <v>0.92794821277793405</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C9" s="39">
         <f>lda!B18</f>
         <v>0.72248803827751196</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D9" s="39">
         <f>lda!B49</f>
         <v>0.79763580073177598</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E9" s="39">
         <f>lda!B73</f>
         <v>0.85702223473121297</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F9" s="39">
         <f>lda!B93</f>
         <v>0.92316352378271904</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C12" s="17">
         <v>14</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D12" s="17">
         <v>8</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E12" s="17">
         <v>7</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F12" s="17">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <f>Lasso!B20</f>
         <v>0.70319061437430497</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <f>Lasso!B51</f>
         <v>0.78167255359736199</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <f>Lasso!B75</f>
         <v>0.84018006845375304</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <f>Lasso!B95</f>
         <v>0.89591152365582105</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <f>mlr!B19</f>
         <v>0.70369582286874199</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <f>mlr!B50</f>
         <v>0.78369196633902205</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="1">
         <f>mlr!B74</f>
         <v>0.84129267322105905</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
         <f>mlr!B94</f>
         <v>0.89681679031729</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1">
+        <f>rfor!B19</f>
+        <v>0.69535284801092001</v>
+      </c>
+      <c r="D15" s="1">
+        <f>rfor!B50</f>
+        <v>0.76171894229421999</v>
+      </c>
+      <c r="E15" s="1">
+        <f>rfor!B73</f>
+        <v>0.835954284425248</v>
+      </c>
+      <c r="F15" s="1">
+        <f>rfor!B93</f>
+        <v>0.88254823663967297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C16" s="1">
         <f>qda!B19</f>
         <v>0.69062779815848496</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D16" s="1">
         <f>qda!B50</f>
         <v>0.76919909175968604</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E16" s="1">
         <f>qda!B74</f>
         <v>0.84387931088331403</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F16" s="1">
         <f>qda!B93</f>
         <v>0.88816695112312005</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C17" s="1">
         <f>svm!B19</f>
         <v>0.67916806658481699</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D17" s="1">
         <f>svm!B50</f>
         <v>0.75955593767277596</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E17" s="1">
         <f>svm!B73</f>
         <v>0.82746927418610805</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F17" s="1">
         <f>svm!B93</f>
         <v>0.88133647797511405</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C18" s="1">
         <f>lda!B19</f>
         <v>0.67011406451690703</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D18" s="1">
         <f>lda!B50</f>
         <v>0.74831160565445098</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E18" s="1">
         <f>lda!B74</f>
         <v>0.80827476349882199</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F18" s="1">
         <f>lda!B94</f>
         <v>0.87408291788022596</v>
       </c>
@@ -2310,7 +2571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
@@ -12237,7 +12498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
@@ -14673,4 +14934,2446 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A78" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="23" customWidth="1"/>
+    <col min="8" max="9" width="10.33203125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="13" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>344</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>44</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0</v>
+      </c>
+      <c r="L2" s="5">
+        <v>2</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>128</v>
+      </c>
+      <c r="E4" s="5">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>1</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1049</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>12</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5</v>
+      </c>
+      <c r="I5" s="5">
+        <v>19</v>
+      </c>
+      <c r="J5" s="5">
+        <v>8</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>26</v>
+      </c>
+      <c r="M5" s="5">
+        <v>11</v>
+      </c>
+      <c r="N5" s="5">
+        <v>4</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5">
+        <v>280</v>
+      </c>
+      <c r="H7" s="5">
+        <v>36</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5">
+        <v>14</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1</v>
+      </c>
+      <c r="L7" s="5">
+        <v>57</v>
+      </c>
+      <c r="M7" s="5">
+        <v>6</v>
+      </c>
+      <c r="N7" s="5">
+        <v>19</v>
+      </c>
+      <c r="O7" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>14</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>9</v>
+      </c>
+      <c r="F8" s="5">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5">
+        <v>28</v>
+      </c>
+      <c r="H8" s="5">
+        <v>330</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2</v>
+      </c>
+      <c r="J8" s="5">
+        <v>7</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>4</v>
+      </c>
+      <c r="M8" s="5">
+        <v>12</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>1</v>
+      </c>
+      <c r="I9" s="5">
+        <v>13</v>
+      </c>
+      <c r="J9" s="5">
+        <v>4</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5">
+        <v>1</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>2</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>4</v>
+      </c>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5">
+        <v>82</v>
+      </c>
+      <c r="L11" s="5">
+        <v>4</v>
+      </c>
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>24</v>
+      </c>
+      <c r="F12" s="5">
+        <v>23</v>
+      </c>
+      <c r="G12" s="5">
+        <v>67</v>
+      </c>
+      <c r="H12" s="5">
+        <v>13</v>
+      </c>
+      <c r="I12" s="5">
+        <v>62</v>
+      </c>
+      <c r="J12" s="5">
+        <v>37</v>
+      </c>
+      <c r="K12" s="5">
+        <v>4</v>
+      </c>
+      <c r="L12" s="5">
+        <v>320</v>
+      </c>
+      <c r="M12" s="5">
+        <v>14</v>
+      </c>
+      <c r="N12" s="5">
+        <v>31</v>
+      </c>
+      <c r="O12" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
+        <v>1</v>
+      </c>
+      <c r="M13" s="5">
+        <v>3</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
+        <v>2</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2</v>
+      </c>
+      <c r="J15" s="5">
+        <v>3</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>4</v>
+      </c>
+      <c r="M15" s="5">
+        <v>5</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.74810019701660602</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.69535284801092001</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" spans="1:15" ht="24" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.98350777037741799</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.86868686868686895</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.98226164079822598</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.99424956871765402</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.71830985915492895</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.99310740953474996</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.99267935578330901</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.83660130718954195</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.997058823529412</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0.91535776614310604</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0.94515995014540899</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.88823031329381896</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.95910623946037099</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6.8965517241379296E-2</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.99885550786838295</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.499999999999998</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.98476727785613505</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.93339676498572799</v>
+      </c>
+      <c r="D27" s="6">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.96082272282076397</v>
+      </c>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.97177291468442795</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.78758949880668205</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.97766432673899195</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="6">
+        <v>0.118181818181818</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.994191112401975</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.39393939393939298</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.97244318181818201</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.6315789473684199E-2</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.99971239574345705</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.66666666666670304</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.97915492957746497</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.93181818181818199</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.99653679653679605</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.87234042553191404</v>
+      </c>
+      <c r="E31" s="6">
+        <v>0.99826539462272301</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.752941176470588</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.90632992327365702</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.52202283849918396</v>
+      </c>
+      <c r="E32" s="6">
+        <v>0.96428571428571397</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="6">
+        <v>5.6603773584905703E-2</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.999428571428571</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.60000000000000597</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.985907553551296</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3.3333333333333298E-2</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0.99914113942170102</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.40000000000000902</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.98365276211950403</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.40322580645161299</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.99066783318751805</v>
+      </c>
+      <c r="D35" s="6">
+        <v>0.60975609756097704</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.97868049553442804</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="26"/>
+      <c r="B38" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="26">
+        <v>344</v>
+      </c>
+      <c r="C39" s="26">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26">
+        <v>6</v>
+      </c>
+      <c r="E39" s="26">
+        <v>44</v>
+      </c>
+      <c r="F39" s="26">
+        <v>0</v>
+      </c>
+      <c r="G39" s="26">
+        <v>0</v>
+      </c>
+      <c r="H39" s="26">
+        <v>2</v>
+      </c>
+      <c r="I39" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="26">
+        <v>0</v>
+      </c>
+      <c r="C40" s="26">
+        <v>51</v>
+      </c>
+      <c r="D40" s="26">
+        <v>0</v>
+      </c>
+      <c r="E40" s="26">
+        <v>2</v>
+      </c>
+      <c r="F40" s="26">
+        <v>1</v>
+      </c>
+      <c r="G40" s="26">
+        <v>14</v>
+      </c>
+      <c r="H40" s="26">
+        <v>3</v>
+      </c>
+      <c r="I40" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="26">
+        <v>16</v>
+      </c>
+      <c r="C41" s="26">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26">
+        <v>128</v>
+      </c>
+      <c r="E41" s="26">
+        <v>8</v>
+      </c>
+      <c r="F41" s="26">
+        <v>0</v>
+      </c>
+      <c r="G41" s="26">
+        <v>0</v>
+      </c>
+      <c r="H41" s="26">
+        <v>1</v>
+      </c>
+      <c r="I41" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="26">
+        <v>40</v>
+      </c>
+      <c r="C42" s="26">
+        <v>2</v>
+      </c>
+      <c r="D42" s="26">
+        <v>4</v>
+      </c>
+      <c r="E42" s="26">
+        <v>1049</v>
+      </c>
+      <c r="F42" s="26">
+        <v>12</v>
+      </c>
+      <c r="G42" s="26">
+        <v>5</v>
+      </c>
+      <c r="H42" s="26">
+        <v>69</v>
+      </c>
+      <c r="I42" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="26">
+        <v>0</v>
+      </c>
+      <c r="C43" s="26">
+        <v>3</v>
+      </c>
+      <c r="D43" s="26">
+        <v>0</v>
+      </c>
+      <c r="E43" s="26">
+        <v>5</v>
+      </c>
+      <c r="F43" s="26">
+        <v>280</v>
+      </c>
+      <c r="G43" s="26">
+        <v>36</v>
+      </c>
+      <c r="H43" s="26">
+        <v>165</v>
+      </c>
+      <c r="I43" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="26">
+        <v>0</v>
+      </c>
+      <c r="C44" s="26">
+        <v>14</v>
+      </c>
+      <c r="D44" s="26">
+        <v>0</v>
+      </c>
+      <c r="E44" s="26">
+        <v>9</v>
+      </c>
+      <c r="F44" s="26">
+        <v>28</v>
+      </c>
+      <c r="G44" s="26">
+        <v>330</v>
+      </c>
+      <c r="H44" s="26">
+        <v>38</v>
+      </c>
+      <c r="I44" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="26">
+        <v>0</v>
+      </c>
+      <c r="C45" s="26">
+        <v>5</v>
+      </c>
+      <c r="D45" s="26">
+        <v>0</v>
+      </c>
+      <c r="E45" s="26">
+        <v>29</v>
+      </c>
+      <c r="F45" s="26">
+        <v>79</v>
+      </c>
+      <c r="G45" s="26">
+        <v>15</v>
+      </c>
+      <c r="H45" s="26">
+        <v>616</v>
+      </c>
+      <c r="I45" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="26">
+        <v>0</v>
+      </c>
+      <c r="C46" s="26">
+        <v>0</v>
+      </c>
+      <c r="D46" s="26">
+        <v>0</v>
+      </c>
+      <c r="E46" s="26">
+        <v>0</v>
+      </c>
+      <c r="F46" s="26">
+        <v>0</v>
+      </c>
+      <c r="G46" s="26">
+        <v>0</v>
+      </c>
+      <c r="H46" s="26">
+        <v>12</v>
+      </c>
+      <c r="I46" s="26">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="26"/>
+      <c r="B48" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="27">
+        <v>0.81058260624824097</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="27">
+        <v>0.76171894229421999</v>
+      </c>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="27">
+        <v>0.86</v>
+      </c>
+      <c r="C53" s="27">
+        <v>0.98350777037741799</v>
+      </c>
+      <c r="D53" s="27">
+        <v>0.86868686868686895</v>
+      </c>
+      <c r="E53" s="27">
+        <v>0.98226164079822598</v>
+      </c>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="27">
+        <v>0.68</v>
+      </c>
+      <c r="C54" s="27">
+        <v>0.99424956871765402</v>
+      </c>
+      <c r="D54" s="27">
+        <v>0.71830985915492895</v>
+      </c>
+      <c r="E54" s="27">
+        <v>0.99310740953474996</v>
+      </c>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="27">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="C55" s="27">
+        <v>0.99267935578330901</v>
+      </c>
+      <c r="D55" s="27">
+        <v>0.83660130718954195</v>
+      </c>
+      <c r="E55" s="27">
+        <v>0.997058823529412</v>
+      </c>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="27">
+        <v>0.91535776614310604</v>
+      </c>
+      <c r="C56" s="27">
+        <v>0.94515995014540899</v>
+      </c>
+      <c r="D56" s="27">
+        <v>0.88823031329381896</v>
+      </c>
+      <c r="E56" s="27">
+        <v>0.95910623946037099</v>
+      </c>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="C57" s="27">
+        <v>0.93339676498572799</v>
+      </c>
+      <c r="D57" s="27">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="E57" s="27">
+        <v>0.96082272282076397</v>
+      </c>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="27">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="C58" s="27">
+        <v>0.97177291468442795</v>
+      </c>
+      <c r="D58" s="27">
+        <v>0.78758949880668205</v>
+      </c>
+      <c r="E58" s="27">
+        <v>0.97766432673899195</v>
+      </c>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="27">
+        <v>0.67991169977924903</v>
+      </c>
+      <c r="C59" s="27">
+        <v>0.94975443898753298</v>
+      </c>
+      <c r="D59" s="27">
+        <v>0.82242990654205606</v>
+      </c>
+      <c r="E59" s="27">
+        <v>0.89657631954350903</v>
+      </c>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="27">
+        <v>0.93181818181818199</v>
+      </c>
+      <c r="C60" s="27">
+        <v>0.99653679653679605</v>
+      </c>
+      <c r="D60" s="27">
+        <v>0.87234042553191404</v>
+      </c>
+      <c r="E60" s="27">
+        <v>0.99826539462272301</v>
+      </c>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="28"/>
+      <c r="B62" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" s="28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="28">
+        <v>344</v>
+      </c>
+      <c r="C63" s="28">
+        <v>0</v>
+      </c>
+      <c r="D63" s="28">
+        <v>6</v>
+      </c>
+      <c r="E63" s="28">
+        <v>44</v>
+      </c>
+      <c r="F63" s="28">
+        <v>0</v>
+      </c>
+      <c r="G63" s="28">
+        <v>2</v>
+      </c>
+      <c r="H63" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="28">
+        <v>0</v>
+      </c>
+      <c r="C64" s="28">
+        <v>51</v>
+      </c>
+      <c r="D64" s="28">
+        <v>0</v>
+      </c>
+      <c r="E64" s="28">
+        <v>2</v>
+      </c>
+      <c r="F64" s="28">
+        <v>14</v>
+      </c>
+      <c r="G64" s="28">
+        <v>4</v>
+      </c>
+      <c r="H64" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" s="28">
+        <v>16</v>
+      </c>
+      <c r="C65" s="28">
+        <v>0</v>
+      </c>
+      <c r="D65" s="28">
+        <v>128</v>
+      </c>
+      <c r="E65" s="28">
+        <v>8</v>
+      </c>
+      <c r="F65" s="28">
+        <v>0</v>
+      </c>
+      <c r="G65" s="28">
+        <v>1</v>
+      </c>
+      <c r="H65" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="28">
+        <v>40</v>
+      </c>
+      <c r="C66" s="28">
+        <v>2</v>
+      </c>
+      <c r="D66" s="28">
+        <v>4</v>
+      </c>
+      <c r="E66" s="28">
+        <v>1049</v>
+      </c>
+      <c r="F66" s="28">
+        <v>5</v>
+      </c>
+      <c r="G66" s="28">
+        <v>81</v>
+      </c>
+      <c r="H66" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="28">
+        <v>0</v>
+      </c>
+      <c r="C67" s="28">
+        <v>14</v>
+      </c>
+      <c r="D67" s="28">
+        <v>0</v>
+      </c>
+      <c r="E67" s="28">
+        <v>9</v>
+      </c>
+      <c r="F67" s="28">
+        <v>330</v>
+      </c>
+      <c r="G67" s="28">
+        <v>66</v>
+      </c>
+      <c r="H67" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="28">
+        <v>0</v>
+      </c>
+      <c r="C68" s="28">
+        <v>8</v>
+      </c>
+      <c r="D68" s="28">
+        <v>0</v>
+      </c>
+      <c r="E68" s="28">
+        <v>34</v>
+      </c>
+      <c r="F68" s="28">
+        <v>51</v>
+      </c>
+      <c r="G68" s="28">
+        <v>1140</v>
+      </c>
+      <c r="H68" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" s="28">
+        <v>0</v>
+      </c>
+      <c r="C69" s="28">
+        <v>0</v>
+      </c>
+      <c r="D69" s="28">
+        <v>0</v>
+      </c>
+      <c r="E69" s="28">
+        <v>0</v>
+      </c>
+      <c r="F69" s="28">
+        <v>0</v>
+      </c>
+      <c r="G69" s="28">
+        <v>12</v>
+      </c>
+      <c r="H69" s="28">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="28"/>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="28"/>
+      <c r="G70" s="28"/>
+      <c r="H70" s="28"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="28"/>
+      <c r="B71" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="28"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="29">
+        <v>0.87925696594427205</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="28"/>
+      <c r="G72" s="28"/>
+      <c r="H72" s="28"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" s="29">
+        <v>0.835954284425248</v>
+      </c>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
+    </row>
+    <row r="74" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G74" s="28"/>
+      <c r="H74" s="28"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="28"/>
+      <c r="B75" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75" s="28"/>
+      <c r="G75" s="28"/>
+      <c r="H75" s="28"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="29">
+        <v>0.86</v>
+      </c>
+      <c r="C76" s="29">
+        <v>0.98350777037741799</v>
+      </c>
+      <c r="D76" s="29">
+        <v>0.86868686868686895</v>
+      </c>
+      <c r="E76" s="29">
+        <v>0.98226164079822598</v>
+      </c>
+      <c r="F76" s="28"/>
+      <c r="G76" s="28"/>
+      <c r="H76" s="28"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="29">
+        <v>0.68</v>
+      </c>
+      <c r="C77" s="29">
+        <v>0.99424956871765402</v>
+      </c>
+      <c r="D77" s="29">
+        <v>0.71830985915492895</v>
+      </c>
+      <c r="E77" s="29">
+        <v>0.99310740953474996</v>
+      </c>
+      <c r="F77" s="28"/>
+      <c r="G77" s="28"/>
+      <c r="H77" s="28"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" s="29">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="C78" s="29">
+        <v>0.99267935578330901</v>
+      </c>
+      <c r="D78" s="29">
+        <v>0.83660130718954195</v>
+      </c>
+      <c r="E78" s="29">
+        <v>0.997058823529412</v>
+      </c>
+      <c r="F78" s="28"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="28"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="29">
+        <v>0.91535776614310604</v>
+      </c>
+      <c r="C79" s="29">
+        <v>0.94515995014540899</v>
+      </c>
+      <c r="D79" s="29">
+        <v>0.88823031329381896</v>
+      </c>
+      <c r="E79" s="29">
+        <v>0.95910623946037099</v>
+      </c>
+      <c r="F79" s="28"/>
+      <c r="G79" s="28"/>
+      <c r="H79" s="28"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="29">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="C80" s="29">
+        <v>0.97177291468442795</v>
+      </c>
+      <c r="D80" s="29">
+        <v>0.78758949880668205</v>
+      </c>
+      <c r="E80" s="29">
+        <v>0.97766432673899195</v>
+      </c>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B81" s="29">
+        <v>0.872894333843798</v>
+      </c>
+      <c r="C81" s="29">
+        <v>0.95594125500667604</v>
+      </c>
+      <c r="D81" s="29">
+        <v>0.92009685230024196</v>
+      </c>
+      <c r="E81" s="29">
+        <v>0.92826274848746804</v>
+      </c>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
+      <c r="H81" s="28"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B82" s="29">
+        <v>0.93181818181818199</v>
+      </c>
+      <c r="C82" s="29">
+        <v>0.99653679653679605</v>
+      </c>
+      <c r="D82" s="29">
+        <v>0.87234042553191404</v>
+      </c>
+      <c r="E82" s="29">
+        <v>0.99826539462272301</v>
+      </c>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="28"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="30"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="30"/>
+      <c r="B85" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B86" s="30">
+        <v>344</v>
+      </c>
+      <c r="C86" s="30">
+        <v>2</v>
+      </c>
+      <c r="D86" s="30">
+        <v>6</v>
+      </c>
+      <c r="E86" s="30">
+        <v>44</v>
+      </c>
+      <c r="F86" s="30"/>
+      <c r="G86" s="30"/>
+      <c r="H86" s="30"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="30">
+        <v>0</v>
+      </c>
+      <c r="C87" s="30">
+        <v>1778</v>
+      </c>
+      <c r="D87" s="30">
+        <v>0</v>
+      </c>
+      <c r="E87" s="30">
+        <v>45</v>
+      </c>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="30">
+        <v>16</v>
+      </c>
+      <c r="C88" s="30">
+        <v>1</v>
+      </c>
+      <c r="D88" s="30">
+        <v>128</v>
+      </c>
+      <c r="E88" s="30">
+        <v>8</v>
+      </c>
+      <c r="F88" s="30"/>
+      <c r="G88" s="30"/>
+      <c r="H88" s="30"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="30">
+        <v>40</v>
+      </c>
+      <c r="C89" s="30">
+        <v>88</v>
+      </c>
+      <c r="D89" s="30">
+        <v>4</v>
+      </c>
+      <c r="E89" s="30">
+        <v>1049</v>
+      </c>
+      <c r="F89" s="30"/>
+      <c r="G89" s="30"/>
+      <c r="H89" s="30"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="30"/>
+      <c r="H90" s="30"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="30"/>
+      <c r="B91" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="30"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="30"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B92" s="31">
+        <v>0.92851111736560699</v>
+      </c>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="30"/>
+      <c r="F92" s="30"/>
+      <c r="G92" s="30"/>
+      <c r="H92" s="30"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" s="31">
+        <v>0.88254823663967297</v>
+      </c>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="30"/>
+      <c r="G93" s="30"/>
+      <c r="H93" s="30"/>
+    </row>
+    <row r="94" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A94" s="30"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="G94" s="30"/>
+      <c r="H94" s="30"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="30"/>
+      <c r="B95" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="30"/>
+      <c r="G95" s="30"/>
+      <c r="H95" s="30"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B96" s="31">
+        <v>0.86</v>
+      </c>
+      <c r="C96" s="31">
+        <v>0.98350777037741799</v>
+      </c>
+      <c r="D96" s="31">
+        <v>0.86868686868686895</v>
+      </c>
+      <c r="E96" s="31">
+        <v>0.98226164079822598</v>
+      </c>
+      <c r="F96" s="30"/>
+      <c r="G96" s="30"/>
+      <c r="H96" s="30"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" s="31">
+        <v>0.95131086142322097</v>
+      </c>
+      <c r="C97" s="31">
+        <v>0.97327790973871697</v>
+      </c>
+      <c r="D97" s="31">
+        <v>0.97531541415249601</v>
+      </c>
+      <c r="E97" s="31">
+        <v>0.947398843930636</v>
+      </c>
+      <c r="F97" s="30"/>
+      <c r="G97" s="30"/>
+      <c r="H97" s="30"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="31">
+        <v>0.92753623188405798</v>
+      </c>
+      <c r="C98" s="31">
+        <v>0.99267935578330901</v>
+      </c>
+      <c r="D98" s="31">
+        <v>0.83660130718954195</v>
+      </c>
+      <c r="E98" s="31">
+        <v>0.997058823529412</v>
+      </c>
+      <c r="F98" s="30"/>
+      <c r="G98" s="30"/>
+      <c r="H98" s="30"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="31">
+        <v>0.91535776614310604</v>
+      </c>
+      <c r="C99" s="31">
+        <v>0.94515995014540899</v>
+      </c>
+      <c r="D99" s="31">
+        <v>0.88823031329381896</v>
+      </c>
+      <c r="E99" s="31">
+        <v>0.95910623946037099</v>
+      </c>
+      <c r="F99" s="30"/>
+      <c r="G99" s="30"/>
+      <c r="H99" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>